<commit_message>
Add bulk insert, erd image, and insert excel file
</commit_message>
<xml_diff>
--- a/Group_2_Insert_Tables.xlsx
+++ b/Group_2_Insert_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bette\Desktop\School\Data\Group Work\doomsday-prep-group-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264FE30B-458F-4405-A760-01836179A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07277CD7-4A2E-423C-B055-38AC2E23305E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28590" yWindow="5220" windowWidth="16410" windowHeight="11055" firstSheet="2" activeTab="6" xr2:uid="{22D6B13A-ECFC-4116-8885-F53E97F37EC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22D6B13A-ECFC-4116-8885-F53E97F37EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="City" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Status" sheetId="7" r:id="rId5"/>
     <sheet name="Survivors" sheetId="1" r:id="rId6"/>
     <sheet name="Skill" sheetId="8" r:id="rId7"/>
-    <sheet name="Look_ups" sheetId="5" r:id="rId8"/>
+    <sheet name="DiseaseCase" sheetId="9" r:id="rId8"/>
+    <sheet name="Look_ups" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="1106">
   <si>
     <t>shelter_id</t>
   </si>
@@ -3356,6 +3357,33 @@
   </si>
   <si>
     <t>The ability to create traps to capture small game.</t>
+  </si>
+  <si>
+    <t>survivor_id</t>
+  </si>
+  <si>
+    <t>diagnosis_date</t>
+  </si>
+  <si>
+    <t>cure_date</t>
+  </si>
+  <si>
+    <t>Earliest Infection</t>
+  </si>
+  <si>
+    <t>Latest Infection</t>
+  </si>
+  <si>
+    <t>power_source_id</t>
+  </si>
+  <si>
+    <t>water_source_id</t>
+  </si>
+  <si>
+    <t>skill_id</t>
+  </si>
+  <si>
+    <t>disease_case_id</t>
   </si>
 </sst>
 </file>
@@ -3734,78 +3762,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C08EC4-F2E0-4DF7-9BC1-ABB516A250FF}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3816,181 +3847,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A56894E-107F-4F4C-9560-2D33DBADE830}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <f ca="1">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C11" ca="1" si="0">RANDBETWEEN(0,1)</f>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" ca="1" si="0">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="C4">
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E10">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="E11">
         <v>0</v>
       </c>
     </row>
@@ -4001,87 +4035,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27CA41F-87F0-4615-9324-D3219D73A9EC}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="str">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
+        <v>Dirty</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
         <v>Prestine</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="str">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
         <v>Dirty</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="str">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
+        <v>Dirty</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
+        <v>Good</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
+        <v>Prestine</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
+        <v>Fine</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
         <v>Bad</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="str">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
         <v>Dirty</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
-        <v>Good</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
-        <v>Prestine</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
-        <v>Toxic</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
-        <v>Toxic</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="str">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
         <v>Bad</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,6),Look_ups!$A$1:$B$7,2,FALSE)</f>
-        <v>Prestine</v>
       </c>
     </row>
   </sheetData>
@@ -4091,195 +4128,198 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE32D69C-02A8-421C-8A34-105575EA5ACD}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
         <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>6</v>
+      </c>
+      <c r="C2" t="str">
+        <f ca="1">VLOOKUP(B2,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Homestead"</f>
+        <v>Provincetown Homestead</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(4,16)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" ref="B3:B13" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <f ca="1">VLOOKUP(B3,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Shelter"</f>
+        <v>Springfield Shelter</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" ca="1" si="1">RANDBETWEEN(4,16)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
-      <c r="B2" t="str">
-        <f ca="1">VLOOKUP(A2,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Homestead"</f>
-        <v>Wareham Homestead</v>
-      </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(4,16)</f>
+      <c r="C4" t="str">
+        <f ca="1">VLOOKUP(B4,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Bunker"</f>
+        <v>Wareham Bunker</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">VLOOKUP(B5,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Bed &amp; Breakfast"</f>
+        <v>Watertown Bed &amp; Breakfast</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">VLOOKUP(B6,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Estate"</f>
+        <v>Wareham Estate</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">VLOOKUP(B7,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Farm"</f>
+        <v>Chatham Farm</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A13" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
-      </c>
-      <c r="B3" t="str">
-        <f ca="1">VLOOKUP(A3,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Shelter"</f>
-        <v>Sandwich Shelter</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C13" ca="1" si="1">RANDBETWEEN(4,16)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B4" t="str">
-        <f ca="1">VLOOKUP(A4,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Bunker"</f>
-        <v>Worcester Bunker</v>
-      </c>
-      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f ca="1">VLOOKUP(B8,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Refuge"</f>
+        <v>Wareham Refuge</v>
+      </c>
+      <c r="D8">
         <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="B5" t="str">
-        <f ca="1">VLOOKUP(A5,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Bed &amp; Breakfast"</f>
-        <v>Provincetown Bed &amp; Breakfast</v>
-      </c>
-      <c r="C5">
+      <c r="C9" t="str">
+        <f ca="1">VLOOKUP(B9,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Cabin"</f>
+        <v>Provincetown Cabin</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C10" t="str">
+        <f ca="1">VLOOKUP(B10,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Depot"</f>
+        <v>Sandwich Depot</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>3</v>
+      </c>
+      <c r="C11" t="str">
+        <f ca="1">VLOOKUP(B11,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Redoubt"</f>
+        <v>Chatham Redoubt</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C12" t="str">
+        <f ca="1">VLOOKUP(B12,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Asylum"</f>
+        <v>Wareham Asylum</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C13" t="str">
+        <f ca="1">VLOOKUP(B13,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Safehouse"</f>
+        <v>Wareham Safehouse</v>
+      </c>
+      <c r="D13">
         <f t="shared" ca="1" si="1"/>
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f ca="1">VLOOKUP(A6,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Estate"</f>
-        <v>Sandwich Estate</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B7" t="str">
-        <f ca="1">VLOOKUP(A7,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Farm"</f>
-        <v>Wareham Farm</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" t="str">
-        <f ca="1">VLOOKUP(A8,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Refuge"</f>
-        <v>Worcester Refuge</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B9" t="str">
-        <f ca="1">VLOOKUP(A9,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Cabin"</f>
-        <v>Springfield Cabin</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B10" t="str">
-        <f ca="1">VLOOKUP(A10,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Depot"</f>
-        <v>Watertown Depot</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
-      </c>
-      <c r="B11" t="str">
-        <f ca="1">VLOOKUP(A11,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Redoubt"</f>
-        <v>Chatham Redoubt</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ca="1" si="1"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B12" t="str">
-        <f ca="1">VLOOKUP(A12,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Asylum"</f>
-        <v>Wareham Asylum</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B13" t="str">
-        <f ca="1">VLOOKUP(A13,Look_ups!$A$1:$C$12,3,FALSE)&amp;" Safehouse"</f>
-        <v>Wareham Safehouse</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -4289,41 +4329,69 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C986B0BA-7DE1-4BEA-8DC2-8B98AC6C133D}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4334,559 +4402,1282 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF24C5A-75AF-48EC-BDEA-8F8C1E2BE2A3}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f t="shared" ref="A2:A30" ca="1" si="0">RANDBETWEEN(1,12)</f>
-        <v>9</v>
-      </c>
-      <c r="B2" t="str">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f t="shared" ref="B2:B65" ca="1" si="0">RANDBETWEEN(1,12)</f>
+        <v>8</v>
+      </c>
+      <c r="C2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Leland</v>
-      </c>
-      <c r="C2" t="str">
+        <v>Valery</v>
+      </c>
+      <c r="D2" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Frye</v>
-      </c>
-      <c r="D2" s="2">
+        <v>Villalobos</v>
+      </c>
+      <c r="E2" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>46570</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+        <v>46400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Rosalee</v>
+      </c>
+      <c r="D3" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Stanley</v>
+      </c>
+      <c r="E3" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>27674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C4" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Omari</v>
+      </c>
+      <c r="D4" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Moyer</v>
+      </c>
+      <c r="E4" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>27751</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Kallie</v>
+      </c>
+      <c r="D5" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Wyatt</v>
+      </c>
+      <c r="E5" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>40785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Allyson</v>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Johnston</v>
+      </c>
+      <c r="E6" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Aron</v>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Aguirre</v>
+      </c>
+      <c r="E7" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>47405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Dangelo</v>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>King</v>
+      </c>
+      <c r="E8" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>36910</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Baker</v>
+      </c>
+      <c r="D9" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Bowers</v>
+      </c>
+      <c r="E9" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>39833</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C10" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Matthias</v>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Costa</v>
+      </c>
+      <c r="E10" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>34241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C11" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Angelica</v>
+      </c>
+      <c r="D11" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Dawson</v>
+      </c>
+      <c r="E11" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>30276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Finley</v>
+      </c>
+      <c r="D12" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Mayo</v>
+      </c>
+      <c r="E12" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>34919</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Felicity</v>
+      </c>
+      <c r="D13" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Hernandez</v>
+      </c>
+      <c r="E13" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>37427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C14" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Rebecca</v>
+      </c>
+      <c r="D14" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Cruz</v>
+      </c>
+      <c r="E14" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C15" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Weston</v>
+      </c>
+      <c r="D15" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Bishop</v>
+      </c>
+      <c r="E15" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>43787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C16" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Kaiser</v>
+      </c>
+      <c r="D16" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Rhodes</v>
+      </c>
+      <c r="E16" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>27492</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C17" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Haylee</v>
+      </c>
+      <c r="D17" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Felix</v>
+      </c>
+      <c r="E17" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>31534</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C18" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Milana</v>
+      </c>
+      <c r="D18" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Carr</v>
+      </c>
+      <c r="E18" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>38135</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C19" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Darren</v>
+      </c>
+      <c r="D19" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Shah</v>
+      </c>
+      <c r="E19" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46383</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C20" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Leo</v>
+      </c>
+      <c r="D20" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Ball</v>
+      </c>
+      <c r="E20" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>23444</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C21" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Lennox</v>
+      </c>
+      <c r="D21" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Oliver</v>
+      </c>
+      <c r="E21" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>30109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C22" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Atticus</v>
+      </c>
+      <c r="D22" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Fitzgerald</v>
+      </c>
+      <c r="E22" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46423</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C23" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Elian</v>
+      </c>
+      <c r="D23" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Archer</v>
+      </c>
+      <c r="E23" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>40161</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C24" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Misael</v>
+      </c>
+      <c r="D24" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Mueller</v>
+      </c>
+      <c r="E24" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>44800</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C25" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Lilyana</v>
+      </c>
+      <c r="D25" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Valentine</v>
+      </c>
+      <c r="E25" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>44410</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C26" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Rome</v>
+      </c>
+      <c r="D26" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Wyatt</v>
+      </c>
+      <c r="E26" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>26717</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C27" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Evangeline</v>
+      </c>
+      <c r="D27" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Freeman</v>
+      </c>
+      <c r="E27" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46638</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C28" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Ander</v>
+      </c>
+      <c r="D28" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Stephenson</v>
+      </c>
+      <c r="E28" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>23847</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C29" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Tucker</v>
+      </c>
+      <c r="D29" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Edwards</v>
+      </c>
+      <c r="E29" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>41916</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C30" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Arthur</v>
+      </c>
+      <c r="D30" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Galindo</v>
+      </c>
+      <c r="E30" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>26346</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C31" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Meghan</v>
+      </c>
+      <c r="D31" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Cisneros</v>
+      </c>
+      <c r="E31" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>23431</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Anderson</v>
+      </c>
+      <c r="D32" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Klein</v>
+      </c>
+      <c r="E32" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>24439</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C33" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Jade</v>
+      </c>
+      <c r="D33" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Preston</v>
+      </c>
+      <c r="E33" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>30446</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C34" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Aurelia</v>
+      </c>
+      <c r="D34" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Dyer</v>
+      </c>
+      <c r="E34" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>25039</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C35" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Harley</v>
+      </c>
+      <c r="D35" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Klein</v>
+      </c>
+      <c r="E35" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>41515</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Lucas</v>
+      </c>
+      <c r="D36" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Kelly</v>
+      </c>
+      <c r="E36" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>43458</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C37" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Khaleesi</v>
+      </c>
+      <c r="D37" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Stark</v>
+      </c>
+      <c r="E37" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>29210</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C38" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Cruz</v>
+      </c>
+      <c r="D38" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Diaz</v>
+      </c>
+      <c r="E38" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>39135</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C39" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Cruz</v>
+      </c>
+      <c r="D39" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Hardin</v>
+      </c>
+      <c r="E39" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>45639</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C40" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Isla</v>
+      </c>
+      <c r="D40" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Bryant</v>
+      </c>
+      <c r="E40" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>46240</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C41" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Paisleigh</v>
+      </c>
+      <c r="D41" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Walker</v>
+      </c>
+      <c r="E41" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>28134</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C42" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Blaine</v>
+      </c>
+      <c r="D42" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Vo</v>
+      </c>
+      <c r="E42" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>38711</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C43" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Isla</v>
+      </c>
+      <c r="D43" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Logan</v>
+      </c>
+      <c r="E43" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>29930</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C44" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Maria</v>
+      </c>
+      <c r="D44" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Blankenship</v>
+      </c>
+      <c r="E44" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>47744</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C45" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Naya</v>
+      </c>
+      <c r="D45" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Arias</v>
+      </c>
+      <c r="E45" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>38818</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C46" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Addilyn</v>
+      </c>
+      <c r="D46" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Moss</v>
+      </c>
+      <c r="E46" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>45066</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Weston</v>
+      </c>
+      <c r="D47" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Chung</v>
+      </c>
+      <c r="E47" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>29303</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C48" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Kallie</v>
+      </c>
+      <c r="D48" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Swanson</v>
+      </c>
+      <c r="E48" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>45494</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C49" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Savanna</v>
+      </c>
+      <c r="D49" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Petersen</v>
+      </c>
+      <c r="E49" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>25024</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C50" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Eliana</v>
+      </c>
+      <c r="D50" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Fields</v>
+      </c>
+      <c r="E50" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>38022</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C51" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Morgan</v>
+      </c>
+      <c r="D51" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Hart</v>
+      </c>
+      <c r="E51" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>30014</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Emberly</v>
+      </c>
+      <c r="D52" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Page</v>
+      </c>
+      <c r="E52" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>31730</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Ayden</v>
+      </c>
+      <c r="D53" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Duffy</v>
+      </c>
+      <c r="E53" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>40499</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Julissa</v>
+      </c>
+      <c r="D54" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Hanna</v>
+      </c>
+      <c r="E54" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>26685</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Tristen</v>
+      </c>
+      <c r="D55" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Ayers</v>
+      </c>
+      <c r="E55" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>33080</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C56" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Dariel</v>
+      </c>
+      <c r="D56" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>West</v>
+      </c>
+      <c r="E56" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>35431</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C57" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Bridget</v>
+      </c>
+      <c r="D57" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Costa</v>
+      </c>
+      <c r="E57" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>40525</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C58" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
         <v>Liv</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D58" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Stuart</v>
-      </c>
-      <c r="D3" s="2">
+        <v>Day</v>
+      </c>
+      <c r="E58" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>32024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <v>25595</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B4" t="str">
+        <v>6</v>
+      </c>
+      <c r="C59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Salem</v>
-      </c>
-      <c r="C4" t="str">
+        <v>Anne</v>
+      </c>
+      <c r="D59" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Diaz</v>
-      </c>
-      <c r="D4" s="2">
+        <v>Roberts</v>
+      </c>
+      <c r="E59" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>29364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B5" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Felix</v>
-      </c>
-      <c r="C5" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Buckley</v>
-      </c>
-      <c r="D5" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>41608</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>31967</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="B6" t="str">
+      <c r="C60" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Peyton</v>
-      </c>
-      <c r="C6" t="str">
+        <v>Alec</v>
+      </c>
+      <c r="D60" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Underwood</v>
-      </c>
-      <c r="D6" s="2">
+        <v>O’Donnell</v>
+      </c>
+      <c r="E60" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>43508</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B7" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Abdullah</v>
-      </c>
-      <c r="C7" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Gibson</v>
-      </c>
-      <c r="D7" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>28507</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B8" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Hamza</v>
-      </c>
-      <c r="C8" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Barber</v>
-      </c>
-      <c r="D8" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>45138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>40598</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61">
         <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
-      <c r="B9" t="str">
+      <c r="C61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Makai</v>
-      </c>
-      <c r="C9" t="str">
+        <v>Bradley</v>
+      </c>
+      <c r="D61" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Salinas</v>
-      </c>
-      <c r="D9" s="2">
+        <v>Archer</v>
+      </c>
+      <c r="E61" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>45687</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>44498</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C62" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Justice</v>
+      </c>
+      <c r="D62" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Bradford</v>
+      </c>
+      <c r="E62" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C63" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
+        <v>Violeta</v>
+      </c>
+      <c r="D63" t="str">
+        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
+        <v>Valentine</v>
+      </c>
+      <c r="E63" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
+        <v>40733</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="B10" t="str">
+      <c r="C64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Calvin</v>
-      </c>
-      <c r="C10" t="str">
+        <v>Beckham</v>
+      </c>
+      <c r="D64" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Mathis</v>
-      </c>
-      <c r="D10" s="2">
+        <v>Harrington</v>
+      </c>
+      <c r="E64" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>32056</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>37618</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="B11" t="str">
+      <c r="C65" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Stephanie</v>
-      </c>
-      <c r="C11" t="str">
+        <v>Maxwell</v>
+      </c>
+      <c r="D65" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Booker</v>
-      </c>
-      <c r="D11" s="2">
+        <v>Estrada</v>
+      </c>
+      <c r="E65" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>27642</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B12" t="str">
+        <v>44135</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f t="shared" ref="B66:B70" ca="1" si="1">RANDBETWEEN(1,12)</f>
+        <v>11</v>
+      </c>
+      <c r="C66" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Aurelia</v>
-      </c>
-      <c r="C12" t="str">
+        <v>Araceli</v>
+      </c>
+      <c r="D66" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Corona</v>
-      </c>
-      <c r="D12" s="2">
+        <v>Sanford</v>
+      </c>
+      <c r="E66" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>46619</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B13" t="str">
+        <v>37849</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Ruben</v>
-      </c>
-      <c r="C13" t="str">
+        <v>Peter</v>
+      </c>
+      <c r="D67" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Frank</v>
-      </c>
-      <c r="D13" s="2">
+        <v>Ibarra</v>
+      </c>
+      <c r="E67" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>30937</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B14" t="str">
+        <v>28335</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Diego</v>
-      </c>
-      <c r="C14" t="str">
+        <v>Allison</v>
+      </c>
+      <c r="D68" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Howell</v>
-      </c>
-      <c r="D14" s="2">
+        <v>Martinez</v>
+      </c>
+      <c r="E68" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>45333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B15" t="str">
+        <v>32283</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Kenzie</v>
-      </c>
-      <c r="C15" t="str">
+        <v>Zendaya</v>
+      </c>
+      <c r="D69" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Murillo</v>
-      </c>
-      <c r="D15" s="2">
+        <v>Davenport</v>
+      </c>
+      <c r="E69" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>23508</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" ca="1" si="0"/>
+        <v>46091</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="B16" t="str">
+      <c r="C70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Henley</v>
-      </c>
-      <c r="C16" t="str">
+        <v>Trevor</v>
+      </c>
+      <c r="D70" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Sherman</v>
-      </c>
-      <c r="D16" s="2">
+        <v>Floyd</v>
+      </c>
+      <c r="E70" s="2">
         <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>36119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B17" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Egypt</v>
-      </c>
-      <c r="C17" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Santana</v>
-      </c>
-      <c r="D17" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B18" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Phillip</v>
-      </c>
-      <c r="C18" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Franklin</v>
-      </c>
-      <c r="D18" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>26351</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B19" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Drake</v>
-      </c>
-      <c r="C19" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Butler</v>
-      </c>
-      <c r="D19" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>22028</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B20" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Tristan</v>
-      </c>
-      <c r="C20" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Dawson</v>
-      </c>
-      <c r="D20" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>46256</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B21" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Kyler</v>
-      </c>
-      <c r="C21" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Holland</v>
-      </c>
-      <c r="D21" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>37765</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B22" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Gatlin</v>
-      </c>
-      <c r="C22" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Vance</v>
-      </c>
-      <c r="D22" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>43179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B23" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Randy</v>
-      </c>
-      <c r="C23" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Strong</v>
-      </c>
-      <c r="D23" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>47064</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B24" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Clara</v>
-      </c>
-      <c r="C24" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Hull</v>
-      </c>
-      <c r="D24" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>31599</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B25" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Matilda</v>
-      </c>
-      <c r="C25" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Ahmed</v>
-      </c>
-      <c r="D25" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>37508</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B26" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Sergio</v>
-      </c>
-      <c r="C26" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Shaw</v>
-      </c>
-      <c r="D26" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>28261</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B27" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Landyn</v>
-      </c>
-      <c r="C27" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Kirk</v>
-      </c>
-      <c r="D27" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>30069</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B28" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Rayden</v>
-      </c>
-      <c r="C28" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Reynolds</v>
-      </c>
-      <c r="D28" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>33393</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B29" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Alonzo</v>
-      </c>
-      <c r="C29" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Roman</v>
-      </c>
-      <c r="D29" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>41888</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B30" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,5,FALSE)</f>
-        <v>Houston</v>
-      </c>
-      <c r="C30" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(0,1000),Look_ups!$A$1:$F$1001,6,FALSE)</f>
-        <v>Roberts</v>
-      </c>
-      <c r="D30" s="2">
-        <f ca="1">RANDBETWEEN(Look_ups!$K$2,Look_ups!$L$2)</f>
-        <v>44021</v>
+        <v>46909</v>
       </c>
     </row>
   </sheetData>
@@ -4896,143 +5687,266 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D5BA00-64A3-4772-979F-016253803027}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B1" t="s">
         <v>1065</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1070</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1081</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1071</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>1082</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1069</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>1072</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1084</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>1067</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>1085</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>1073</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>1086</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>1074</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>1075</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>1088</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>1076</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>1089</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>1077</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>1090</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>1078</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>1091</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>1079</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>1093</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>1092</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>1094</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>1080</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>1096</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>1068</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>1095</v>
       </c>
     </row>
@@ -5042,11 +5956,329 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CC425C-E6E1-497C-805D-D2C90DAAF68A}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(1,5)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46998</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f ca="1">IF(C2+RANDBETWEEN(20,40)*RANDBETWEEN(0,1)=C2,"",C2+RANDBETWEEN(20,40))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f ca="1">B2+RANDBETWEEN(1,5)</f>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>45911</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f t="shared" ref="D3:D17" ca="1" si="0">IF(C3+RANDBETWEEN(20,40)*RANDBETWEEN(0,1)=C3,"",C3+RANDBETWEEN(20,40))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" ref="B4:B11" ca="1" si="1">B3+RANDBETWEEN(1,5)</f>
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46449</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46146</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>45836</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>45921</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47067</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C9" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47092</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47475</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46393</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" ref="B12:B17" ca="1" si="2">B11+RANDBETWEEN(1,5)</f>
+        <v>30</v>
+      </c>
+      <c r="C12" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47566</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47563</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>47587</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="C14" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46009</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46071</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="C16" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>46525</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" ca="1" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="C17" s="2">
+        <f ca="1">RANDBETWEEN(Look_ups!$M$2,Look_ups!$N$2)</f>
+        <v>47465</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>47486</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53C9114-DF26-4993-9F22-BE9C5B027365}">
-  <dimension ref="A1:L1001"/>
+  <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A970" workbookViewId="0">
-      <selection activeCell="A1002" sqref="A1002"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5055,10 +6287,12 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -5083,8 +6317,14 @@
       <c r="L1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5110,8 +6350,14 @@
       <c r="L2" s="2">
         <v>47848</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="2">
+        <v>45658</v>
+      </c>
+      <c r="N2" s="2">
+        <v>47848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5132,7 +6378,7 @@
         <v>Love</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5153,7 +6399,7 @@
         <v>Carpenter</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5174,7 +6420,7 @@
         <v>Nava</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5195,7 +6441,7 @@
         <v>Vo</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5216,7 +6462,7 @@
         <v>Leach</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5234,7 +6480,7 @@
         <v>Hamilton</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5249,7 +6495,7 @@
         <v>Shepard</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5264,7 +6510,7 @@
         <v>Vaughn</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5279,7 +6525,7 @@
         <v>Cline</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5294,7 +6540,7 @@
         <v>Coleman</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5309,7 +6555,7 @@
         <v>Boyer</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5324,7 +6570,7 @@
         <v>Wu</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5339,7 +6585,7 @@
         <v>McDaniel</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>